<commit_message>
avec smartphone stockage en décimale : 15.5GB + maj library
</commit_message>
<xml_diff>
--- a/testsunitaires/pc_V3_jeu test 2 lignes.xlsx
+++ b/testsunitaires/pc_V3_jeu test 2 lignes.xlsx
@@ -1387,9 +1387,9 @@
   <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="2040" topLeftCell="A216" activePane="bottomLeft" state="split"/>
+      <pane xSplit="0" ySplit="2040" topLeftCell="A1" activePane="bottomLeft" state="split"/>
       <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomLeft" activeCell="P229" activeCellId="0" sqref="P229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>